<commit_message>
Updated PV1033 test scripts
</commit_message>
<xml_diff>
--- a/PSPSProject/testData/dm_Valid_Invalid_Circuits.xlsx
+++ b/PSPSProject/testData/dm_Valid_Invalid_Circuits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PSPSViewerV4.0_GIT\gis-geomartcloud-pspsv4-automation-python\PSPSProject\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286C165B-F4FA-4AFA-BC38-6C8CD77F94D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D67C90-D0A9-43AF-94AF-3BCA7BAAFD31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="765" firstSheet="8" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="765" firstSheet="9" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fail1_EmptyFile" sheetId="1" r:id="rId1"/>
@@ -30,13 +30,14 @@
     <sheet name="Fail15" sheetId="46" r:id="rId15"/>
     <sheet name="Fail16" sheetId="47" r:id="rId16"/>
     <sheet name="Error_Message" sheetId="29" r:id="rId17"/>
+    <sheet name="Success" sheetId="48" r:id="rId18"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="68">
   <si>
     <t>FIA</t>
   </si>
@@ -152,12 +153,6 @@
     <t>EAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDEAST GRANDvv</t>
   </si>
   <si>
-    <t>substation cannot be more than 50 characters</t>
-  </si>
-  <si>
-    <t>substation cannot be null</t>
-  </si>
-  <si>
     <t>Source Is.D Type</t>
   </si>
   <si>
@@ -186,6 +181,66 @@
   </si>
   <si>
     <t>RIO DEL MAR</t>
+  </si>
+  <si>
+    <t>Substation cannot be more than 50 characters</t>
+  </si>
+  <si>
+    <t>Substation cannot be null</t>
+  </si>
+  <si>
+    <t>Test@123</t>
+  </si>
+  <si>
+    <t>130;112</t>
+  </si>
+  <si>
+    <t>ROB ROY 2105</t>
+  </si>
+  <si>
+    <t>ALTO 60KV</t>
+  </si>
+  <si>
+    <t>BIG RIVER 1101</t>
+  </si>
+  <si>
+    <t>BIG RIVER 12.5KV</t>
+  </si>
+  <si>
+    <t>GREENBRAE 1104</t>
+  </si>
+  <si>
+    <t>circuit123</t>
+  </si>
+  <si>
+    <t>circuitname</t>
+  </si>
+  <si>
+    <t>LOW GAP 1101</t>
+  </si>
+  <si>
+    <t>LOW GAP 115KV</t>
+  </si>
+  <si>
+    <t>AUBERRY 1101</t>
+  </si>
+  <si>
+    <t>AUBERRY</t>
+  </si>
+  <si>
+    <t>NARROWS 2101</t>
+  </si>
+  <si>
+    <t>NARROWS</t>
+  </si>
+  <si>
+    <t>ARCATA 1121</t>
+  </si>
+  <si>
+    <t>ARCATA</t>
+  </si>
+  <si>
+    <t>test@123</t>
   </si>
 </sst>
 </file>
@@ -1041,7 +1096,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1357,7 +1412,7 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1449,7 +1504,7 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1530,7 +1585,7 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1622,7 +1677,7 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1668,7 +1723,7 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -1691,7 +1746,7 @@
         <v>28</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
@@ -1732,8 +1787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5163C0BE-8992-4571-B383-28856CA78E1B}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1766,16 +1821,16 @@
         <v>83260401</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2">
         <v>3174</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1788,7 +1843,7 @@
   <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1853,37 +1908,359 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C858F70B-3106-4AAA-8B10-AFFA587840DD}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>123456789</v>
+      </c>
+      <c r="B2">
+        <v>14161105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3">
+        <v>13921102</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>192401101</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>3174</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>190</v>
+      </c>
+      <c r="B5">
+        <v>83692105</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5">
+        <v>11377</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>140</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>140</v>
+      </c>
+      <c r="B7">
+        <v>43081101</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>190</v>
+      </c>
+      <c r="B8">
+        <v>42271105</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8">
+        <v>1619</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>130</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9">
+        <v>192411101</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>130</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10">
+        <v>192411101</v>
+      </c>
+      <c r="D10">
+        <v>4167</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>428</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11">
+        <v>254151101</v>
+      </c>
+      <c r="D11">
+        <v>1284</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>428</v>
+      </c>
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12">
+        <v>254151101</v>
+      </c>
+      <c r="D12">
+        <v>6722</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>300</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13">
+        <v>153132101</v>
+      </c>
+      <c r="E13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>300</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14">
+        <v>153132101</v>
+      </c>
+      <c r="D14">
+        <v>7589</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>100</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15">
+        <v>192021121</v>
+      </c>
+      <c r="D15">
+        <v>5789</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{0211BED1-02E6-4FA3-A439-BD79C92C9154}"/>
+    <hyperlink ref="F8" r:id="rId2" xr:uid="{25EC8A75-100B-4CB7-AB75-31D60E82F1B3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1892,7 +2269,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F4"/>
+      <selection activeCell="A2" sqref="A2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>